<commit_message>
Updated till week 10
</commit_message>
<xml_diff>
--- a/src/menus/NUS Menu Wk 1-8 2019.xlsx
+++ b/src/menus/NUS Menu Wk 1-8 2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ping\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwk97\OneDrive\Desktop\EusoffBot\eusofftelebot\src\menus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7720313C-BFDC-442D-BDB2-A3F87ECB1800}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7720313C-BFDC-442D-BDB2-A3F87ECB1800}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F659406F-16E5-4309-B76F-A14AF5D64138}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3640" yWindow="3370" windowWidth="14400" windowHeight="7090" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -1528,57 +1528,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1596,6 +1545,90 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1605,21 +1638,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1638,20 +1656,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1659,13 +1665,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1991,21 +1991,21 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
     <col min="3" max="3" width="71" style="12" customWidth="1"/>
     <col min="4" max="4" width="78" style="12" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="67.81640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="65" style="12" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="68.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="63.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="65.54296875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="68.7265625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2034,82 +2034,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="75" t="s">
         <v>91</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
+    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51" t="s">
+    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="67"/>
+      <c r="B6" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="64" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="67"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="67"/>
       <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
@@ -2133,9 +2133,9 @@
       </c>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="51" t="s">
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="67"/>
+      <c r="B9" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -2158,9 +2158,9 @@
       </c>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="52"/>
+    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="68"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -2191,7 +2191,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="1"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -2201,8 +2201,8 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2228,8 +2228,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -2253,8 +2253,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -2278,8 +2278,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -2303,9 +2303,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="70"/>
+      <c r="B17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -2328,9 +2328,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="59"/>
+    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="70"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
@@ -2351,9 +2351,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="60"/>
+    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="10" t="s">
         <v>31</v>
       </c>
@@ -2374,55 +2374,55 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="51" t="s">
+    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="14"/>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="70"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="54"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="I21" s="64"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="55"/>
-    </row>
-    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="I22" s="65"/>
+    </row>
+    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="70"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -2446,8 +2446,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="70"/>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -2471,8 +2471,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
+    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="70"/>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
@@ -2496,8 +2496,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="71"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B27" s="6"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -2531,7 +2531,7 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -2557,15 +2557,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A13:A26"/>
     <mergeCell ref="B9:B10"/>
@@ -2582,6 +2573,15 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="43" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2599,21 +2599,21 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
     <col min="3" max="3" width="71" style="12" customWidth="1"/>
     <col min="4" max="4" width="78" style="12" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="76.453125" style="12" customWidth="1"/>
     <col min="6" max="6" width="65" style="12" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="68.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="63.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="65.54296875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="68.7265625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>198</v>
       </c>
@@ -2642,82 +2642,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="75" t="s">
         <v>98</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
+    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51" t="s">
+    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="67"/>
+      <c r="B6" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="64" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="67"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="67"/>
       <c r="B8" s="30" t="s">
         <v>25</v>
       </c>
@@ -2741,9 +2741,9 @@
       </c>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="51" t="s">
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="67"/>
+      <c r="B9" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -2766,9 +2766,9 @@
       </c>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="52"/>
+    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="68"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="29" t="s">
         <v>15</v>
       </c>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -2799,7 +2799,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="1"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -2809,8 +2809,8 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2836,8 +2836,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -2861,8 +2861,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -2886,8 +2886,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -2911,9 +2911,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="70"/>
+      <c r="B17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -2936,9 +2936,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="59"/>
+    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="70"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="4" t="s">
         <v>123</v>
       </c>
@@ -2959,9 +2959,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="60"/>
+    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="27" t="s">
         <v>127</v>
       </c>
@@ -2982,55 +2982,55 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="51" t="s">
+    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="28"/>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="70"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="54"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="I21" s="64"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="55"/>
-    </row>
-    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="I22" s="65"/>
+    </row>
+    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="70"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -3054,8 +3054,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="70"/>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -3079,8 +3079,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
+    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="70"/>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
@@ -3104,8 +3104,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="71"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B27" s="6"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -3139,7 +3139,7 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -3165,15 +3165,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="A13:A26"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="B6:B7"/>
@@ -3184,12 +3181,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="A13:A26"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="43" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3203,25 +3203,25 @@
   </sheetPr>
   <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
     <col min="3" max="3" width="71" style="12" customWidth="1"/>
     <col min="4" max="4" width="78" style="12" customWidth="1"/>
-    <col min="5" max="5" width="83.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="83.26953125" style="12" customWidth="1"/>
     <col min="6" max="6" width="65" style="12" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="74.7109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="68.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="63.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="74.7265625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="68.7265625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>199</v>
       </c>
@@ -3250,82 +3250,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="75" t="s">
         <v>91</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
+    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51" t="s">
+    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="67"/>
+      <c r="B6" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="64" t="s">
         <v>150</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="67"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="67"/>
       <c r="B8" s="30" t="s">
         <v>25</v>
       </c>
@@ -3349,9 +3349,9 @@
       </c>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="51" t="s">
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="67"/>
+      <c r="B9" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -3374,9 +3374,9 @@
       </c>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="52"/>
+    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="68"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="29" t="s">
         <v>15</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -3407,7 +3407,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="1"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -3417,8 +3417,8 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -3444,8 +3444,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+    <row r="14" spans="1:9" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -3469,8 +3469,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -3494,8 +3494,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -3519,9 +3519,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="70"/>
+      <c r="B17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -3544,9 +3544,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="59"/>
+    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="70"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="4" t="s">
         <v>162</v>
       </c>
@@ -3567,9 +3567,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="60"/>
+    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="27" t="s">
         <v>166</v>
       </c>
@@ -3590,55 +3590,55 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="51" t="s">
+    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="28"/>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="70"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="54"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="I21" s="64"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="55"/>
-    </row>
-    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="I22" s="65"/>
+    </row>
+    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="70"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -3662,8 +3662,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="70"/>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -3687,8 +3687,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
+    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="70"/>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
@@ -3712,8 +3712,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="71"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B27" s="6"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -3747,7 +3747,7 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -3773,15 +3773,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="A13:A26"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="B6:B7"/>
@@ -3792,12 +3789,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="A13:A26"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="43" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3811,25 +3811,25 @@
   </sheetPr>
   <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
     <col min="3" max="3" width="71" style="12" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="71.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="68.7265625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="71.54296875" style="12" customWidth="1"/>
     <col min="6" max="6" width="65" style="12" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="63.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="65.54296875" style="12" customWidth="1"/>
     <col min="9" max="9" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>174</v>
       </c>
@@ -3854,86 +3854,86 @@
       <c r="H3" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="45" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="75" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="63"/>
-    </row>
-    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51" t="s">
+      <c r="I4" s="46"/>
+    </row>
+    <row r="5" spans="1:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="46"/>
+    </row>
+    <row r="6" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="67"/>
+      <c r="B6" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="75" t="s">
         <v>179</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="61" t="s">
+      <c r="H6" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="63"/>
-    </row>
-    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="63"/>
-    </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="I6" s="46"/>
+    </row>
+    <row r="7" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="67"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="1:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="67"/>
       <c r="B8" s="30" t="s">
         <v>25</v>
       </c>
@@ -3955,11 +3955,11 @@
       <c r="H8" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="63"/>
-    </row>
-    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="51" t="s">
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="67"/>
+      <c r="B9" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -3980,11 +3980,11 @@
       <c r="H9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="63"/>
-    </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="52"/>
+      <c r="I9" s="46"/>
+    </row>
+    <row r="10" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="68"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="29" t="s">
         <v>15</v>
       </c>
@@ -4003,9 +4003,9 @@
       <c r="H10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="64"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -4014,7 +4014,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="1"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -4023,8 +4023,8 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -4046,12 +4046,12 @@
         <v>1</v>
       </c>
       <c r="H13" s="27"/>
-      <c r="I13" s="65" t="s">
+      <c r="I13" s="48" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+    <row r="14" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -4071,12 +4071,12 @@
         <v>186</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="65" t="s">
+      <c r="I14" s="48" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+    <row r="15" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -4096,12 +4096,12 @@
         <v>189</v>
       </c>
       <c r="H15" s="28"/>
-      <c r="I15" s="66" t="s">
+      <c r="I15" s="49" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+    <row r="16" spans="1:9" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -4121,13 +4121,13 @@
         <v>35</v>
       </c>
       <c r="H16" s="28"/>
-      <c r="I16" s="65" t="s">
+      <c r="I16" s="48" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:9" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="70"/>
+      <c r="B17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -4146,13 +4146,13 @@
         <v>36</v>
       </c>
       <c r="H17" s="28"/>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="50" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="59"/>
+    <row r="18" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="70"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="4" t="s">
         <v>123</v>
       </c>
@@ -4169,13 +4169,13 @@
         <v>70</v>
       </c>
       <c r="H18" s="28"/>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="48" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="60"/>
+    <row r="19" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="27" t="s">
         <v>127</v>
       </c>
@@ -4192,59 +4192,59 @@
         <v>131</v>
       </c>
       <c r="H19" s="28"/>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="51" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="51" t="s">
+    <row r="20" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="28"/>
-      <c r="I20" s="69" t="s">
+      <c r="I20" s="80" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="70"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="70"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="I21" s="81"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="71"/>
-    </row>
-    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="I22" s="82"/>
+    </row>
+    <row r="23" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="70"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -4264,12 +4264,12 @@
         <v>136</v>
       </c>
       <c r="H23" s="28"/>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="51" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
+    <row r="24" spans="1:9" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="70"/>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -4289,12 +4289,12 @@
         <v>197</v>
       </c>
       <c r="H24" s="28"/>
-      <c r="I24" s="74" t="s">
+      <c r="I24" s="54" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
+    <row r="25" spans="1:9" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="70"/>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
@@ -4314,12 +4314,12 @@
         <v>34</v>
       </c>
       <c r="H25" s="28"/>
-      <c r="I25" s="65" t="s">
+      <c r="I25" s="48" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="71"/>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
@@ -4339,11 +4339,11 @@
         <v>22</v>
       </c>
       <c r="H26" s="29"/>
-      <c r="I26" s="65" t="s">
+      <c r="I26" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B27" s="6"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -4352,7 +4352,7 @@
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -4363,7 +4363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -4376,15 +4376,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="A13:A26"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="B6:B7"/>
@@ -4395,12 +4392,15 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="A13:A26"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="43" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4415,20 +4415,20 @@
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="71" style="12" customWidth="1"/>
-    <col min="4" max="4" width="70.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="69.42578125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="66.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="54.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="70.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="69.453125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="66.26953125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="64.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="54.1796875" style="12" customWidth="1"/>
     <col min="9" max="9" width="60" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>320</v>
       </c>
@@ -4457,82 +4457,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="75" t="s">
         <v>91</v>
       </c>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+    <row r="3" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="67"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="58" t="s">
+    <row r="4" spans="1:9" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="67"/>
+      <c r="B4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="64" t="s">
         <v>321</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="64" t="s">
         <v>322</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
+    <row r="5" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+    <row r="6" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="67"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -4556,9 +4556,9 @@
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="51" t="s">
+    <row r="7" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="67"/>
+      <c r="B7" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -4581,9 +4581,9 @@
       </c>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47"/>
-      <c r="B8" s="52"/>
+    <row r="8" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="68"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
@@ -4602,9 +4602,9 @@
       <c r="H8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="87"/>
-    </row>
-    <row r="9" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="61"/>
+    </row>
+    <row r="9" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="1"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -4614,327 +4614,327 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="68"/>
-      <c r="I10" s="65" t="s">
+      <c r="H10" s="51"/>
+      <c r="I10" s="48" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="75" t="s">
+    <row r="11" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="70"/>
+      <c r="B11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="65" t="s">
+      <c r="H11" s="56"/>
+      <c r="I11" s="48" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="75" t="s">
+    <row r="12" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
+      <c r="B12" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="48" t="s">
         <v>222</v>
       </c>
-      <c r="G12" s="65" t="s">
+      <c r="G12" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="73" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="53" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="75" t="s">
+    <row r="13" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="70"/>
+      <c r="B13" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="D13" s="65" t="s">
+      <c r="D13" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="65" t="s">
+      <c r="G13" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="H13" s="72"/>
-      <c r="I13" s="65" t="s">
+      <c r="H13" s="52"/>
+      <c r="I13" s="48" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="77" t="s">
+    <row r="14" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
+      <c r="B14" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="48" t="s">
         <v>230</v>
       </c>
-      <c r="H14" s="72"/>
-      <c r="I14" s="65" t="s">
+      <c r="H14" s="52"/>
+      <c r="I14" s="48" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="65" t="s">
+    <row r="15" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="H15" s="72"/>
-      <c r="I15" s="73" t="s">
+      <c r="H15" s="52"/>
+      <c r="I15" s="53" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="68" t="s">
+    <row r="16" spans="1:9" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="G16" s="67" t="s">
+      <c r="G16" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72" t="s">
+      <c r="H16" s="52"/>
+      <c r="I16" s="52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="80" t="s">
+    <row r="17" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="69" t="s">
+      <c r="F17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="69" t="s">
+      <c r="G17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="72"/>
-      <c r="I17" s="69" t="s">
+      <c r="H17" s="52"/>
+      <c r="I17" s="80" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="70"/>
-    </row>
-    <row r="19" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="71"/>
-    </row>
-    <row r="20" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="75" t="s">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="70"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="81"/>
+    </row>
+    <row r="19" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="82"/>
+    </row>
+    <row r="20" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="70"/>
+      <c r="B20" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="48" t="s">
         <v>239</v>
       </c>
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="65" t="s">
+      <c r="F20" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="48" t="s">
         <v>240</v>
       </c>
-      <c r="H20" s="72"/>
-      <c r="I20" s="65" t="s">
+      <c r="H20" s="52"/>
+      <c r="I20" s="48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="83" t="s">
+    <row r="21" spans="1:9" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="70"/>
+      <c r="B21" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="D21" s="85" t="s">
+      <c r="D21" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="E21" s="85" t="s">
+      <c r="E21" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="F21" s="85" t="s">
+      <c r="F21" s="59" t="s">
         <v>245</v>
       </c>
-      <c r="G21" s="85" t="s">
+      <c r="G21" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="85" t="s">
+      <c r="H21" s="52"/>
+      <c r="I21" s="59" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="75" t="s">
+    <row r="22" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
+      <c r="B22" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="F22" s="65" t="s">
+      <c r="F22" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="65" t="s">
+      <c r="G22" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="H22" s="72"/>
-      <c r="I22" s="65" t="s">
+      <c r="H22" s="52"/>
+      <c r="I22" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="75" t="s">
+    <row r="23" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="71"/>
+      <c r="B23" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="65" t="s">
+      <c r="G23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="73"/>
-      <c r="I23" s="65" t="s">
+      <c r="H23" s="53"/>
+      <c r="I23" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="6"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -4944,20 +4944,11 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="86"/>
+    <row r="25" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F25" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="I17:I19"/>
@@ -4974,6 +4965,15 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4988,20 +4988,20 @@
       <selection activeCell="A10" sqref="A10:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="59.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="56.140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="51.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="53.7265625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="63.7265625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="59.7265625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="59.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="56.1796875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="41.26953125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="51.7265625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>323</v>
       </c>
@@ -5030,82 +5030,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="75" t="s">
         <v>98</v>
       </c>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+    <row r="3" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="91"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="58" t="s">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="91"/>
+      <c r="B4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="64" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="H4" s="89" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="57"/>
+    <row r="5" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="91"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+    <row r="6" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="91"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -5129,9 +5129,9 @@
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="51" t="s">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="91"/>
+      <c r="B7" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -5154,9 +5154,9 @@
       </c>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
-      <c r="B8" s="52"/>
+    <row r="8" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="92"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
@@ -5177,9 +5177,9 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+    <row r="9" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -5205,8 +5205,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+    <row r="11" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="70"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5230,8 +5230,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -5255,8 +5255,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="70"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -5280,9 +5280,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="58" t="s">
+    <row r="14" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
+      <c r="B14" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="33" t="s">
@@ -5305,9 +5305,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="59"/>
+    <row r="15" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="42" t="s">
         <v>32</v>
       </c>
@@ -5328,9 +5328,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
+    <row r="16" spans="1:9" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="40" t="s">
         <v>267</v>
       </c>
@@ -5351,55 +5351,55 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="51" t="s">
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="61" t="s">
+      <c r="G17" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="41"/>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="70"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="54"/>
-    </row>
-    <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="I18" s="64"/>
+    </row>
+    <row r="19" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
+      <c r="I19" s="65"/>
+    </row>
+    <row r="20" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="70"/>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -5423,8 +5423,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+    <row r="21" spans="1:9" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="70"/>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
@@ -5448,8 +5448,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
+    <row r="22" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -5473,8 +5473,8 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="71"/>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B24" s="6"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5508,7 +5508,7 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B25" s="6"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5520,15 +5520,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="I17:I19"/>
@@ -5545,6 +5536,15 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5558,20 +5558,20 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" style="12" customWidth="1"/>
     <col min="4" max="4" width="59" style="12" customWidth="1"/>
-    <col min="5" max="5" width="56.140625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="50.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="50.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="56.1796875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="50.26953125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="50.81640625" style="12" customWidth="1"/>
     <col min="8" max="8" width="22" style="12" customWidth="1"/>
     <col min="9" max="9" width="53" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>325</v>
       </c>
@@ -5600,82 +5600,82 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="75" t="s">
         <v>91</v>
       </c>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+    <row r="3" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="91"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="58" t="s">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="91"/>
+      <c r="B4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="H4" s="89" t="s">
         <v>150</v>
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="57"/>
+    <row r="5" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="91"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
+    <row r="6" spans="1:9" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="91"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -5694,14 +5694,14 @@
       <c r="G6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="62" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="51" t="s">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="91"/>
+      <c r="B7" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -5724,9 +5724,9 @@
       </c>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
-      <c r="B8" s="52"/>
+    <row r="8" spans="1:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="92"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
@@ -5747,9 +5747,9 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -5775,8 +5775,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+    <row r="11" spans="1:9" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="70"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5800,8 +5800,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+    <row r="12" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -5825,8 +5825,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="70"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -5850,9 +5850,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="58" t="s">
+    <row r="14" spans="1:9" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
+      <c r="B14" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -5875,9 +5875,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="59"/>
+    <row r="15" spans="1:9" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="4" t="s">
         <v>42</v>
       </c>
@@ -5898,9 +5898,9 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
+    <row r="16" spans="1:9" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="40" t="s">
         <v>31</v>
       </c>
@@ -5921,55 +5921,55 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="51" t="s">
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="61" t="s">
+      <c r="G17" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="41"/>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="70"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="54"/>
-    </row>
-    <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="I18" s="64"/>
+    </row>
+    <row r="19" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
+      <c r="I19" s="65"/>
+    </row>
+    <row r="20" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="70"/>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -5993,8 +5993,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+    <row r="21" spans="1:9" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="70"/>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
@@ -6018,8 +6018,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
+    <row r="22" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -6043,8 +6043,8 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="71"/>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B24" s="6"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -6078,7 +6078,7 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B25" s="6"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -6088,7 +6088,7 @@
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B26" s="6"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -6100,15 +6100,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="I17:I19"/>
@@ -6125,6 +6116,15 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6138,20 +6138,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="53.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="46.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="53.26953125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="55.26953125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="53.26953125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="36.81640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="46.81640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>326</v>
       </c>
@@ -6176,86 +6176,86 @@
       <c r="H1" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="45" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="75" t="s">
         <v>176</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="63"/>
-    </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="63"/>
-    </row>
-    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="58" t="s">
+      <c r="I2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="67"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="46"/>
+    </row>
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="67"/>
+      <c r="B4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="75" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="75" t="s">
         <v>327</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="63"/>
-    </row>
-    <row r="5" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="I4" s="46"/>
+    </row>
+    <row r="5" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="67"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="46"/>
+    </row>
+    <row r="6" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="67"/>
       <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
@@ -6277,11 +6277,11 @@
       <c r="H6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="63"/>
-    </row>
-    <row r="7" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="51" t="s">
+      <c r="I6" s="46"/>
+    </row>
+    <row r="7" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="67"/>
+      <c r="B7" s="72" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -6302,11 +6302,11 @@
       <c r="H7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="63"/>
-    </row>
-    <row r="8" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47"/>
-      <c r="B8" s="52"/>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="68"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
@@ -6325,9 +6325,9 @@
       <c r="H8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="64"/>
-    </row>
-    <row r="9" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="47"/>
+    </row>
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="1"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -6337,8 +6337,8 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -6364,8 +6364,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+    <row r="11" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="70"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -6389,8 +6389,8 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+    <row r="12" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -6414,8 +6414,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+    <row r="13" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="70"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -6439,9 +6439,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="58" t="s">
+    <row r="14" spans="1:9" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="70"/>
+      <c r="B14" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -6464,9 +6464,9 @@
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="59"/>
+    <row r="15" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="70"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="4" t="s">
         <v>123</v>
       </c>
@@ -6487,9 +6487,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
+    <row r="16" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="70"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="40" t="s">
         <v>127</v>
       </c>
@@ -6510,55 +6510,55 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="51" t="s">
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="70"/>
+      <c r="B17" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="61" t="s">
+      <c r="G17" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="41"/>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="63" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="70"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="54"/>
-    </row>
-    <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="I18" s="64"/>
+    </row>
+    <row r="19" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
+      <c r="I19" s="65"/>
+    </row>
+    <row r="20" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="70"/>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
@@ -6582,8 +6582,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+    <row r="21" spans="1:9" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="70"/>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
@@ -6607,8 +6607,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
+    <row r="22" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="70"/>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -6632,8 +6632,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="71"/>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="B24" s="6"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -6669,6 +6669,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="A10:A23"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B4:B5"/>
@@ -6678,22 +6693,7 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="A10:A23"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>